<commit_message>
added outlier testing pipelines
</commit_message>
<xml_diff>
--- a/BERTopic/tasks/output/results-camelbert-seed10-summary.xlsx
+++ b/BERTopic/tasks/output/results-camelbert-seed10-summary.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Github-repos\topic-modeling-tests\BERTopic\tasks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005997BF-7F52-40D3-93CD-6F51CAC8C96D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D13E597D-CF80-4E3E-B959-AF24728F2F64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results-camelbert-seed10-summar" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16694" uniqueCount="11514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16743" uniqueCount="11530">
   <si>
     <t>Topic</t>
   </si>
@@ -34562,6 +34563,54 @@
   </si>
   <si>
     <t>اعجميا</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> تبثيا قال تقول لا تنم بحديثنا ولا تبثه علي الناس وعن قولها ولا تنقث ميرتنا تنقيثا قال تقول لا تسرق ميرتنا ولا تقبضه والميره ما يمتارون من الطعام قال اخوه يوسف في كتاب الله ونمير اهلنا والميره ما يمتارون من الطعام وغيره لا ياخذ منه شيا وعن قولها ولا تملا بيتنا تعشيشا قال تقول نظيفه تنظف البيت وتقمه ولا تدع </t>
+  </si>
+  <si>
+    <t>0281IbnDizilHamdani.Juz.Shamela0026740-ara1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> والطا من قولهم فراش وط بين الوطا والوعا وعا الحمل من متاع كان او غيره قال الله جل ثناه فبدا باوعيتهم قبل وعا اخيه ثم استخرجها من وعا اخيه سوره يوسف وكل ظرف جعلت فيه شيا فذلك الظرف وعاه وصدر الرجل وعا علمه والكا السير والخيط الذي يشد به السقا وغيره يقال اوكيت الش اوكيه ايكا والش الذي يشد به </t>
+  </si>
+  <si>
+    <t>0356AbuCaliQali.MaqsurWaMamdud.Sham19Y0020949-ara1</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Quote</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> خضره حلوه لانهما جعلتا نعتين للدنيا فجرتا علي ظاهر الكلام قال صاحب كتاب العين الرتع الاكل والشرب رغدا في الريف ولا يكون الرتع الا في الخصب والسعه كما قال اخوه يوسف ص نرتع ونلعب وتقول رتع فلان في مال فلان اذا انقلب فيه اكلا وشربا وقال الفرزدق ارعي فزاره لا هناك المرتع وقال ابا جعفر لما توليت ارتعوا وقالوا لدنياهم </t>
+  </si>
+  <si>
+    <t>0360Ramhurmuzi.AmthalHadith.Shia002175-ara1</t>
+  </si>
+  <si>
+    <t>Ref with direct allusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ولاتعجيف قال التعجيف ان ينقل قوتها الي غيرها قبل ان تشبع من الجدوبه قال والعجوف منع النفس من المقابح والعجوف ايضا ترك الطعام وقول الله جل وعز ياكلهن سبع عجاف يوسف هي الهزلي التي لا لحم عليها ولا شحم ضربت مثلا بسبع سنين لا قطر فيها ولا خصب عفج ابو عبيد عن ابي زيد الاعفاج للانسان واحدها عفج والمصارين لذوات </t>
+  </si>
+  <si>
+    <t>0370AbuMansurAzhari.TahdhibLugha.JK007040-ara1</t>
+  </si>
+  <si>
+    <t>Ref - abstained from food</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الاصمعي ناقه شفوع تجمع بين محلبين في حلبه وهي القرون وشفعه الضحي ركعتا الضحي جا في الحديث شعف قال الله جل وعز قد شغفها حبا انا لنراها في ضلال مبين يوسف وقد قري الحرف بالعين والغين فاخبرني المنذري عن الحسين بن فهم عن محمد بن سلام عن يونس انه قال من قراها شعفها حبا فمعناه تيمها ومن قراها شغفها يوسف </t>
+  </si>
+  <si>
+    <t>Allusion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الحراني عن ابن السكيت انه قال شعفه الحب اذا بلغ منه وفلان مشعوف بفلانه وقد شعفه حبها ويقال شعف الهنا البعير اذا بلغ منه المه وقال الفرا في قوله شغفها يوسف زعموا ان الحسن كان يقرا بها قال وهو من قوله شعفت بها كانه قد ذهب بها كل مذهب والشعف روس الجبال وقال ابو عبيد الشعف بالعين احراق الحب القلب </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> في السما كانه سدي ارجوان واستقلت عبورها ابو عبيد عن ابي عبيده المعصب الذي عصبته السنون اي اكلت ماله وقال الله جل وعز ونحن عصبه ان ابانا لفي ضلال مبين يوسف قال ابو عبيد قال ابو زيد العصبه من العشره الي الاربعين وقال الاخفش العصبه والعصابه جماعه ليس لها واحد وذكر ابن المظفر في كتابه حديثا انه يكون في اخر </t>
   </si>
 </sst>
 </file>
@@ -35474,8 +35523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1669"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -108919,4 +108968,310 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65650E94-C7E2-4B28-81EB-7D2B9474F38A}">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11514</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11515</v>
+      </c>
+      <c r="C1">
+        <v>22</v>
+      </c>
+      <c r="D1">
+        <v>24</v>
+      </c>
+      <c r="E1">
+        <v>527</v>
+      </c>
+      <c r="F1" t="s">
+        <v>246</v>
+      </c>
+      <c r="G1" t="s">
+        <v>247</v>
+      </c>
+      <c r="H1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I1" t="s">
+        <v>249</v>
+      </c>
+      <c r="J1">
+        <v>445</v>
+      </c>
+      <c r="K1">
+        <v>124</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11518</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11516</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11517</v>
+      </c>
+      <c r="C2">
+        <v>211</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+      <c r="E2">
+        <v>527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" t="s">
+        <v>247</v>
+      </c>
+      <c r="H2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I2" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2">
+        <v>445</v>
+      </c>
+      <c r="K2">
+        <v>124</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11519</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11520</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11521</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>527</v>
+      </c>
+      <c r="F3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G3" t="s">
+        <v>247</v>
+      </c>
+      <c r="H3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J3">
+        <v>445</v>
+      </c>
+      <c r="K3">
+        <v>124</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>11522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11523</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11524</v>
+      </c>
+      <c r="C4">
+        <v>258</v>
+      </c>
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>527</v>
+      </c>
+      <c r="F4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H4" t="s">
+        <v>248</v>
+      </c>
+      <c r="I4" t="s">
+        <v>249</v>
+      </c>
+      <c r="J4">
+        <v>445</v>
+      </c>
+      <c r="K4">
+        <v>124</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>11525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11526</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11524</v>
+      </c>
+      <c r="C5">
+        <v>294</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5">
+        <v>527</v>
+      </c>
+      <c r="F5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H5" t="s">
+        <v>248</v>
+      </c>
+      <c r="I5" t="s">
+        <v>249</v>
+      </c>
+      <c r="J5">
+        <v>445</v>
+      </c>
+      <c r="K5">
+        <v>124</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11527</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11528</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11524</v>
+      </c>
+      <c r="C6">
+        <v>294</v>
+      </c>
+      <c r="D6">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>527</v>
+      </c>
+      <c r="F6" t="s">
+        <v>246</v>
+      </c>
+      <c r="G6" t="s">
+        <v>247</v>
+      </c>
+      <c r="H6" t="s">
+        <v>248</v>
+      </c>
+      <c r="I6" t="s">
+        <v>249</v>
+      </c>
+      <c r="J6">
+        <v>445</v>
+      </c>
+      <c r="K6">
+        <v>124</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11527</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11529</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11524</v>
+      </c>
+      <c r="C7">
+        <v>359</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>527</v>
+      </c>
+      <c r="F7" t="s">
+        <v>246</v>
+      </c>
+      <c r="G7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I7" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7">
+        <v>445</v>
+      </c>
+      <c r="K7">
+        <v>124</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>11519</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>